<commit_message>
demo app load from labels
</commit_message>
<xml_diff>
--- a/parameters_processingtime.xlsx
+++ b/parameters_processingtime.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
   <si>
     <t>slope</t>
   </si>
@@ -36,9 +36,6 @@
     <t>IMG_5820.MOV</t>
   </si>
   <si>
-    <t>1920x1080</t>
-  </si>
-  <si>
     <t>1687931809010.MP4</t>
   </si>
   <si>
@@ -46,6 +43,21 @@
   </si>
   <si>
     <t>result/s</t>
+  </si>
+  <si>
+    <t>2536187151918482376.mp4</t>
+  </si>
+  <si>
+    <t>IMG_0421</t>
+  </si>
+  <si>
+    <t>450x854</t>
+  </si>
+  <si>
+    <t>1080x1920</t>
+  </si>
+  <si>
+    <t>750x1400</t>
   </si>
 </sst>
 </file>
@@ -67,7 +79,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,6 +101,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -157,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,6 +184,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -192,19 +225,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -487,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM16"/>
+  <dimension ref="A1:AM28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,11 +525,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>5</v>
+      <c r="A1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -620,8 +644,8 @@
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="10"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
@@ -735,8 +759,8 @@
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="10"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
@@ -850,55 +874,117 @@
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="13">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5">
         <v>708</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="E4" s="17">
+        <v>571</v>
+      </c>
+      <c r="F4" s="17">
+        <v>572</v>
+      </c>
+      <c r="G4" s="17">
+        <v>499</v>
+      </c>
+      <c r="H4" s="17">
+        <v>476</v>
+      </c>
+      <c r="I4" s="17">
+        <v>469</v>
+      </c>
+      <c r="J4" s="17">
+        <v>463</v>
+      </c>
+      <c r="K4" s="17">
+        <v>400</v>
+      </c>
+      <c r="L4" s="17">
+        <v>372</v>
+      </c>
+      <c r="M4" s="17">
+        <v>369</v>
+      </c>
+      <c r="N4" s="17">
+        <v>370</v>
+      </c>
       <c r="O4" s="2"/>
       <c r="P4" s="3"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="17">
+        <v>560</v>
+      </c>
+      <c r="S4" s="3">
+        <v>491</v>
+      </c>
       <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
+      <c r="U4" s="17">
+        <v>523</v>
+      </c>
+      <c r="V4" s="17">
+        <v>456</v>
+      </c>
+      <c r="W4" s="17">
+        <v>391</v>
+      </c>
       <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2"/>
-      <c r="AG4" s="2"/>
-      <c r="AH4" s="2"/>
-      <c r="AI4" s="2"/>
-      <c r="AJ4" s="2"/>
-      <c r="AK4" s="2"/>
-      <c r="AL4" s="2"/>
-      <c r="AM4" s="2"/>
+      <c r="Y4" s="17">
+        <v>428</v>
+      </c>
+      <c r="Z4" s="17">
+        <v>430</v>
+      </c>
+      <c r="AA4" s="17">
+        <v>477</v>
+      </c>
+      <c r="AB4" s="17">
+        <v>604</v>
+      </c>
+      <c r="AC4" s="17">
+        <v>566</v>
+      </c>
+      <c r="AD4" s="17">
+        <v>567</v>
+      </c>
+      <c r="AE4" s="17">
+        <v>478</v>
+      </c>
+      <c r="AF4" s="17">
+        <v>533</v>
+      </c>
+      <c r="AG4" s="17">
+        <v>540</v>
+      </c>
+      <c r="AH4" s="17">
+        <v>539</v>
+      </c>
+      <c r="AI4" s="17">
+        <v>470</v>
+      </c>
+      <c r="AJ4" s="17">
+        <v>511</v>
+      </c>
+      <c r="AK4" s="17">
+        <v>511</v>
+      </c>
+      <c r="AL4" s="17">
+        <v>460</v>
+      </c>
+      <c r="AM4" s="17">
+        <v>458</v>
+      </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1012,8 +1098,8 @@
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1127,8 +1213,8 @@
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1242,81 +1328,81 @@
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="13">
+        <v>7</v>
+      </c>
+      <c r="D8" s="17">
         <v>85</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="18">
         <v>92</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="17">
         <v>87</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="17">
         <v>89</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="17">
         <v>85</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="17">
         <v>87</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="17">
         <v>82</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="17">
         <v>94</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="17">
         <v>82</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="17">
         <v>84</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="17">
         <v>80</v>
       </c>
-      <c r="O8" s="13">
+      <c r="O8" s="17">
         <v>78</v>
       </c>
-      <c r="P8" s="13">
+      <c r="P8" s="17">
         <v>110</v>
       </c>
-      <c r="Q8" s="13">
+      <c r="Q8" s="17">
         <v>111</v>
       </c>
-      <c r="R8" s="13">
+      <c r="R8" s="17">
         <v>106</v>
       </c>
-      <c r="S8" s="13">
+      <c r="S8" s="17">
         <v>114</v>
       </c>
-      <c r="T8" s="13">
+      <c r="T8" s="17">
         <v>108</v>
       </c>
-      <c r="U8" s="13">
+      <c r="U8" s="17">
         <v>110</v>
       </c>
-      <c r="V8" s="13">
+      <c r="V8" s="17">
         <v>105</v>
       </c>
-      <c r="W8" s="13">
+      <c r="W8" s="17">
         <v>106</v>
       </c>
-      <c r="X8" s="13">
+      <c r="X8" s="17">
         <v>106</v>
       </c>
-      <c r="Y8" s="13">
+      <c r="Y8" s="17">
         <v>108</v>
       </c>
-      <c r="Z8" s="13">
+      <c r="Z8" s="17">
         <v>109</v>
       </c>
-      <c r="AA8" s="13">
+      <c r="AA8" s="17">
         <v>101</v>
       </c>
       <c r="AB8" s="3"/>
@@ -1333,10 +1419,12 @@
       <c r="AM8" s="3"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="5"/>
+      <c r="A9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
@@ -1450,8 +1538,8 @@
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1565,8 +1653,8 @@
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
@@ -1680,54 +1768,124 @@
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="16"/>
-      <c r="V12" s="16"/>
-      <c r="W12" s="16"/>
-      <c r="X12" s="16"/>
-      <c r="Y12" s="16"/>
-      <c r="Z12" s="16"/>
-      <c r="AA12" s="16"/>
-      <c r="AB12" s="16"/>
-      <c r="AC12" s="16"/>
-      <c r="AD12" s="16"/>
-      <c r="AE12" s="16"/>
-      <c r="AF12" s="16"/>
-      <c r="AG12" s="16"/>
-      <c r="AH12" s="16"/>
-      <c r="AI12" s="16"/>
-      <c r="AJ12" s="16"/>
-      <c r="AK12" s="16"/>
-      <c r="AL12" s="16"/>
-      <c r="AM12" s="16"/>
+        <v>7</v>
+      </c>
+      <c r="D12" s="18">
+        <v>100</v>
+      </c>
+      <c r="E12" s="17">
+        <v>105</v>
+      </c>
+      <c r="F12" s="17">
+        <v>129</v>
+      </c>
+      <c r="G12" s="17">
+        <v>100</v>
+      </c>
+      <c r="H12" s="17">
+        <v>110</v>
+      </c>
+      <c r="I12" s="17">
+        <v>112</v>
+      </c>
+      <c r="J12" s="17">
+        <v>110</v>
+      </c>
+      <c r="K12" s="17">
+        <v>104</v>
+      </c>
+      <c r="L12" s="17">
+        <v>106</v>
+      </c>
+      <c r="M12" s="17">
+        <v>108</v>
+      </c>
+      <c r="N12" s="17">
+        <v>107</v>
+      </c>
+      <c r="O12" s="17">
+        <v>99</v>
+      </c>
+      <c r="P12" s="18">
+        <v>136</v>
+      </c>
+      <c r="Q12" s="17">
+        <v>143</v>
+      </c>
+      <c r="R12" s="17">
+        <v>150</v>
+      </c>
+      <c r="S12" s="17">
+        <v>119</v>
+      </c>
+      <c r="T12" s="17">
+        <v>139</v>
+      </c>
+      <c r="U12" s="17">
+        <v>136</v>
+      </c>
+      <c r="V12" s="17">
+        <v>120</v>
+      </c>
+      <c r="W12" s="17">
+        <v>112</v>
+      </c>
+      <c r="X12" s="17">
+        <v>123</v>
+      </c>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="17">
+        <v>122</v>
+      </c>
+      <c r="AA12" s="17">
+        <v>109</v>
+      </c>
+      <c r="AB12" s="17">
+        <v>184</v>
+      </c>
+      <c r="AC12" s="17">
+        <v>185</v>
+      </c>
+      <c r="AD12" s="17">
+        <v>175</v>
+      </c>
+      <c r="AE12" s="17">
+        <v>170</v>
+      </c>
+      <c r="AF12" s="17">
+        <v>182</v>
+      </c>
+      <c r="AG12" s="17">
+        <v>178</v>
+      </c>
+      <c r="AH12" s="17">
+        <v>171</v>
+      </c>
+      <c r="AI12" s="17">
+        <v>155</v>
+      </c>
+      <c r="AJ12" s="17">
+        <v>178</v>
+      </c>
+      <c r="AK12" s="17">
+        <v>210</v>
+      </c>
+      <c r="AL12" s="17">
+        <v>163</v>
+      </c>
+      <c r="AM12" s="3">
+        <v>156</v>
+      </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>5</v>
+      <c r="A13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>0</v>
@@ -1842,8 +2000,8 @@
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="2" t="s">
         <v>1</v>
       </c>
@@ -1957,8 +2115,8 @@
       </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="6"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
@@ -2072,70 +2230,1258 @@
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4">
+        <v>461</v>
+      </c>
+      <c r="E16" s="5">
+        <v>488</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5">
+        <v>461</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="5">
+        <v>456</v>
+      </c>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="4">
+        <v>558</v>
+      </c>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="5">
+        <v>531</v>
+      </c>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="5">
+        <v>513</v>
+      </c>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="5">
+        <v>591</v>
+      </c>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="6"/>
+      <c r="AF16" s="5">
+        <v>607</v>
+      </c>
+      <c r="AG16" s="6"/>
+      <c r="AH16" s="6"/>
+      <c r="AI16" s="6"/>
+      <c r="AJ16" s="5">
+        <v>581</v>
+      </c>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="6"/>
+      <c r="AM16" s="6"/>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="12">
-        <v>461</v>
-      </c>
-      <c r="E16" s="13">
-        <v>488</v>
-      </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="13">
-        <v>461</v>
-      </c>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="13">
-        <v>456</v>
-      </c>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="12">
-        <v>558</v>
-      </c>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="13">
-        <v>531</v>
-      </c>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
-      <c r="W16" s="14"/>
-      <c r="X16" s="13">
-        <v>513</v>
-      </c>
-      <c r="Y16" s="14"/>
-      <c r="Z16" s="14"/>
-      <c r="AA16" s="14"/>
-      <c r="AB16" s="13">
-        <v>591</v>
-      </c>
-      <c r="AC16" s="14"/>
-      <c r="AD16" s="14"/>
-      <c r="AE16" s="14"/>
-      <c r="AF16" s="13">
-        <v>607</v>
-      </c>
-      <c r="AG16" s="14"/>
-      <c r="AH16" s="14"/>
-      <c r="AI16" s="14"/>
-      <c r="AJ16" s="13">
-        <v>581</v>
-      </c>
-      <c r="AK16" s="14"/>
-      <c r="AL16" s="14"/>
-      <c r="AM16" s="14"/>
+      <c r="B17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="P17" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="R17" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="S17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="T17" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="U17" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="V17" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="W17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="X17" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="Y17" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="Z17" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AA17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AB17" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="AC17" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="AD17" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AE17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AF17" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="AG17" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="AH17" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AI17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AJ17" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="AK17" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="AL17" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AM17" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2">
+        <v>6</v>
+      </c>
+      <c r="F18" s="2">
+        <v>6</v>
+      </c>
+      <c r="G18" s="2">
+        <v>6</v>
+      </c>
+      <c r="H18" s="2">
+        <v>5</v>
+      </c>
+      <c r="I18" s="2">
+        <v>5</v>
+      </c>
+      <c r="J18" s="2">
+        <v>5</v>
+      </c>
+      <c r="K18" s="2">
+        <v>5</v>
+      </c>
+      <c r="L18" s="2">
+        <v>4</v>
+      </c>
+      <c r="M18" s="2">
+        <v>4</v>
+      </c>
+      <c r="N18" s="2">
+        <v>4</v>
+      </c>
+      <c r="O18" s="2">
+        <v>4</v>
+      </c>
+      <c r="P18" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>6</v>
+      </c>
+      <c r="R18" s="2">
+        <v>6</v>
+      </c>
+      <c r="S18" s="2">
+        <v>6</v>
+      </c>
+      <c r="T18" s="2">
+        <v>5</v>
+      </c>
+      <c r="U18" s="2">
+        <v>5</v>
+      </c>
+      <c r="V18" s="2">
+        <v>5</v>
+      </c>
+      <c r="W18" s="2">
+        <v>5</v>
+      </c>
+      <c r="X18" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y18" s="2">
+        <v>4</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>4</v>
+      </c>
+      <c r="AA18" s="2">
+        <v>4</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>6</v>
+      </c>
+      <c r="AC18" s="2">
+        <v>6</v>
+      </c>
+      <c r="AD18" s="2">
+        <v>6</v>
+      </c>
+      <c r="AE18" s="2">
+        <v>6</v>
+      </c>
+      <c r="AF18" s="2">
+        <v>5</v>
+      </c>
+      <c r="AG18" s="2">
+        <v>5</v>
+      </c>
+      <c r="AH18" s="2">
+        <v>5</v>
+      </c>
+      <c r="AI18" s="2">
+        <v>5</v>
+      </c>
+      <c r="AJ18" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK18" s="2">
+        <v>4</v>
+      </c>
+      <c r="AL18" s="2">
+        <v>4</v>
+      </c>
+      <c r="AM18" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2">
+        <v>40</v>
+      </c>
+      <c r="E19" s="2">
+        <v>40</v>
+      </c>
+      <c r="F19" s="2">
+        <v>40</v>
+      </c>
+      <c r="G19" s="2">
+        <v>40</v>
+      </c>
+      <c r="H19" s="2">
+        <v>40</v>
+      </c>
+      <c r="I19" s="2">
+        <v>40</v>
+      </c>
+      <c r="J19" s="2">
+        <v>40</v>
+      </c>
+      <c r="K19" s="2">
+        <v>40</v>
+      </c>
+      <c r="L19" s="2">
+        <v>40</v>
+      </c>
+      <c r="M19" s="2">
+        <v>40</v>
+      </c>
+      <c r="N19" s="2">
+        <v>40</v>
+      </c>
+      <c r="O19" s="2">
+        <v>40</v>
+      </c>
+      <c r="P19" s="2">
+        <v>30</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>30</v>
+      </c>
+      <c r="R19" s="2">
+        <v>30</v>
+      </c>
+      <c r="S19" s="2">
+        <v>30</v>
+      </c>
+      <c r="T19" s="2">
+        <v>30</v>
+      </c>
+      <c r="U19" s="2">
+        <v>30</v>
+      </c>
+      <c r="V19" s="2">
+        <v>30</v>
+      </c>
+      <c r="W19" s="2">
+        <v>30</v>
+      </c>
+      <c r="X19" s="2">
+        <v>30</v>
+      </c>
+      <c r="Y19" s="2">
+        <v>30</v>
+      </c>
+      <c r="Z19" s="2">
+        <v>30</v>
+      </c>
+      <c r="AA19" s="2">
+        <v>30</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC19" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD19" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE19" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF19" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG19" s="2">
+        <v>20</v>
+      </c>
+      <c r="AH19" s="2">
+        <v>20</v>
+      </c>
+      <c r="AI19" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ19" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK19" s="2">
+        <v>20</v>
+      </c>
+      <c r="AL19" s="2">
+        <v>20</v>
+      </c>
+      <c r="AM19" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A20" s="9"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="17">
+        <v>32</v>
+      </c>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="8"/>
+      <c r="AA20" s="8"/>
+      <c r="AB20" s="8"/>
+      <c r="AC20" s="8"/>
+      <c r="AD20" s="8"/>
+      <c r="AE20" s="8"/>
+      <c r="AF20" s="8"/>
+      <c r="AG20" s="8"/>
+      <c r="AH20" s="8"/>
+      <c r="AI20" s="8"/>
+      <c r="AJ20" s="8"/>
+      <c r="AK20" s="8"/>
+      <c r="AL20" s="8"/>
+      <c r="AM20" s="8"/>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M21" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="N21" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="O21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="P21" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="R21" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="S21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="T21" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="U21" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="V21" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="W21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="X21" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="Y21" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="Z21" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AA21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AB21" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="AC21" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="AD21" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AE21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AF21" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="AG21" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="AH21" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AI21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AJ21" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="AK21" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="AL21" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AM21" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A22" s="9"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>6</v>
+      </c>
+      <c r="E22" s="2">
+        <v>6</v>
+      </c>
+      <c r="F22" s="2">
+        <v>6</v>
+      </c>
+      <c r="G22" s="2">
+        <v>6</v>
+      </c>
+      <c r="H22" s="2">
+        <v>5</v>
+      </c>
+      <c r="I22" s="2">
+        <v>5</v>
+      </c>
+      <c r="J22" s="2">
+        <v>5</v>
+      </c>
+      <c r="K22" s="2">
+        <v>5</v>
+      </c>
+      <c r="L22" s="2">
+        <v>4</v>
+      </c>
+      <c r="M22" s="2">
+        <v>4</v>
+      </c>
+      <c r="N22" s="2">
+        <v>4</v>
+      </c>
+      <c r="O22" s="2">
+        <v>4</v>
+      </c>
+      <c r="P22" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>6</v>
+      </c>
+      <c r="R22" s="2">
+        <v>6</v>
+      </c>
+      <c r="S22" s="2">
+        <v>6</v>
+      </c>
+      <c r="T22" s="2">
+        <v>5</v>
+      </c>
+      <c r="U22" s="2">
+        <v>5</v>
+      </c>
+      <c r="V22" s="2">
+        <v>5</v>
+      </c>
+      <c r="W22" s="2">
+        <v>5</v>
+      </c>
+      <c r="X22" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y22" s="2">
+        <v>4</v>
+      </c>
+      <c r="Z22" s="2">
+        <v>4</v>
+      </c>
+      <c r="AA22" s="2">
+        <v>4</v>
+      </c>
+      <c r="AB22" s="2">
+        <v>6</v>
+      </c>
+      <c r="AC22" s="2">
+        <v>6</v>
+      </c>
+      <c r="AD22" s="2">
+        <v>6</v>
+      </c>
+      <c r="AE22" s="2">
+        <v>6</v>
+      </c>
+      <c r="AF22" s="2">
+        <v>5</v>
+      </c>
+      <c r="AG22" s="2">
+        <v>5</v>
+      </c>
+      <c r="AH22" s="2">
+        <v>5</v>
+      </c>
+      <c r="AI22" s="2">
+        <v>5</v>
+      </c>
+      <c r="AJ22" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK22" s="2">
+        <v>4</v>
+      </c>
+      <c r="AL22" s="2">
+        <v>4</v>
+      </c>
+      <c r="AM22" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2">
+        <v>40</v>
+      </c>
+      <c r="E23" s="2">
+        <v>40</v>
+      </c>
+      <c r="F23" s="2">
+        <v>40</v>
+      </c>
+      <c r="G23" s="2">
+        <v>40</v>
+      </c>
+      <c r="H23" s="2">
+        <v>40</v>
+      </c>
+      <c r="I23" s="2">
+        <v>40</v>
+      </c>
+      <c r="J23" s="2">
+        <v>40</v>
+      </c>
+      <c r="K23" s="2">
+        <v>40</v>
+      </c>
+      <c r="L23" s="2">
+        <v>40</v>
+      </c>
+      <c r="M23" s="2">
+        <v>40</v>
+      </c>
+      <c r="N23" s="2">
+        <v>40</v>
+      </c>
+      <c r="O23" s="2">
+        <v>40</v>
+      </c>
+      <c r="P23" s="2">
+        <v>30</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>30</v>
+      </c>
+      <c r="R23" s="2">
+        <v>30</v>
+      </c>
+      <c r="S23" s="2">
+        <v>30</v>
+      </c>
+      <c r="T23" s="2">
+        <v>30</v>
+      </c>
+      <c r="U23" s="2">
+        <v>30</v>
+      </c>
+      <c r="V23" s="2">
+        <v>30</v>
+      </c>
+      <c r="W23" s="2">
+        <v>30</v>
+      </c>
+      <c r="X23" s="2">
+        <v>30</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>30</v>
+      </c>
+      <c r="Z23" s="2">
+        <v>30</v>
+      </c>
+      <c r="AA23" s="2">
+        <v>30</v>
+      </c>
+      <c r="AB23" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC23" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD23" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE23" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF23" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG23" s="2">
+        <v>20</v>
+      </c>
+      <c r="AH23" s="2">
+        <v>20</v>
+      </c>
+      <c r="AI23" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ23" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK23" s="2">
+        <v>20</v>
+      </c>
+      <c r="AL23" s="2">
+        <v>20</v>
+      </c>
+      <c r="AM23" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="17">
+        <v>243</v>
+      </c>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
+      <c r="Y24" s="8"/>
+      <c r="Z24" s="8"/>
+      <c r="AA24" s="8"/>
+      <c r="AB24" s="8"/>
+      <c r="AC24" s="8"/>
+      <c r="AD24" s="8"/>
+      <c r="AE24" s="8"/>
+      <c r="AF24" s="8"/>
+      <c r="AG24" s="8"/>
+      <c r="AH24" s="8"/>
+      <c r="AI24" s="8"/>
+      <c r="AJ24" s="8"/>
+      <c r="AK24" s="8"/>
+      <c r="AL24" s="8"/>
+      <c r="AM24" s="8"/>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="N25" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="O25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="P25" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="R25" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="S25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="T25" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="U25" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="V25" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="W25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="X25" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="Y25" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="Z25" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AA25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AB25" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="AC25" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="AD25" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AE25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AF25" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="AG25" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="AH25" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AI25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AJ25" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="AK25" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="AL25" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AM25" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A26" s="9"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2">
+        <v>6</v>
+      </c>
+      <c r="E26" s="2">
+        <v>6</v>
+      </c>
+      <c r="F26" s="2">
+        <v>6</v>
+      </c>
+      <c r="G26" s="2">
+        <v>6</v>
+      </c>
+      <c r="H26" s="2">
+        <v>5</v>
+      </c>
+      <c r="I26" s="2">
+        <v>5</v>
+      </c>
+      <c r="J26" s="2">
+        <v>5</v>
+      </c>
+      <c r="K26" s="2">
+        <v>5</v>
+      </c>
+      <c r="L26" s="2">
+        <v>4</v>
+      </c>
+      <c r="M26" s="2">
+        <v>4</v>
+      </c>
+      <c r="N26" s="2">
+        <v>4</v>
+      </c>
+      <c r="O26" s="2">
+        <v>4</v>
+      </c>
+      <c r="P26" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>6</v>
+      </c>
+      <c r="R26" s="2">
+        <v>6</v>
+      </c>
+      <c r="S26" s="2">
+        <v>6</v>
+      </c>
+      <c r="T26" s="2">
+        <v>5</v>
+      </c>
+      <c r="U26" s="2">
+        <v>5</v>
+      </c>
+      <c r="V26" s="2">
+        <v>5</v>
+      </c>
+      <c r="W26" s="2">
+        <v>5</v>
+      </c>
+      <c r="X26" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y26" s="2">
+        <v>4</v>
+      </c>
+      <c r="Z26" s="2">
+        <v>4</v>
+      </c>
+      <c r="AA26" s="2">
+        <v>4</v>
+      </c>
+      <c r="AB26" s="2">
+        <v>6</v>
+      </c>
+      <c r="AC26" s="2">
+        <v>6</v>
+      </c>
+      <c r="AD26" s="2">
+        <v>6</v>
+      </c>
+      <c r="AE26" s="2">
+        <v>6</v>
+      </c>
+      <c r="AF26" s="2">
+        <v>5</v>
+      </c>
+      <c r="AG26" s="2">
+        <v>5</v>
+      </c>
+      <c r="AH26" s="2">
+        <v>5</v>
+      </c>
+      <c r="AI26" s="2">
+        <v>5</v>
+      </c>
+      <c r="AJ26" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK26" s="2">
+        <v>4</v>
+      </c>
+      <c r="AL26" s="2">
+        <v>4</v>
+      </c>
+      <c r="AM26" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2">
+        <v>40</v>
+      </c>
+      <c r="E27" s="2">
+        <v>40</v>
+      </c>
+      <c r="F27" s="2">
+        <v>40</v>
+      </c>
+      <c r="G27" s="2">
+        <v>40</v>
+      </c>
+      <c r="H27" s="2">
+        <v>40</v>
+      </c>
+      <c r="I27" s="2">
+        <v>40</v>
+      </c>
+      <c r="J27" s="2">
+        <v>40</v>
+      </c>
+      <c r="K27" s="2">
+        <v>40</v>
+      </c>
+      <c r="L27" s="2">
+        <v>40</v>
+      </c>
+      <c r="M27" s="2">
+        <v>40</v>
+      </c>
+      <c r="N27" s="2">
+        <v>40</v>
+      </c>
+      <c r="O27" s="2">
+        <v>40</v>
+      </c>
+      <c r="P27" s="2">
+        <v>30</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>30</v>
+      </c>
+      <c r="R27" s="2">
+        <v>30</v>
+      </c>
+      <c r="S27" s="2">
+        <v>30</v>
+      </c>
+      <c r="T27" s="2">
+        <v>30</v>
+      </c>
+      <c r="U27" s="2">
+        <v>30</v>
+      </c>
+      <c r="V27" s="2">
+        <v>30</v>
+      </c>
+      <c r="W27" s="2">
+        <v>30</v>
+      </c>
+      <c r="X27" s="2">
+        <v>30</v>
+      </c>
+      <c r="Y27" s="2">
+        <v>30</v>
+      </c>
+      <c r="Z27" s="2">
+        <v>30</v>
+      </c>
+      <c r="AA27" s="2">
+        <v>30</v>
+      </c>
+      <c r="AB27" s="2">
+        <v>20</v>
+      </c>
+      <c r="AC27" s="2">
+        <v>20</v>
+      </c>
+      <c r="AD27" s="2">
+        <v>20</v>
+      </c>
+      <c r="AE27" s="2">
+        <v>20</v>
+      </c>
+      <c r="AF27" s="2">
+        <v>20</v>
+      </c>
+      <c r="AG27" s="2">
+        <v>20</v>
+      </c>
+      <c r="AH27" s="2">
+        <v>20</v>
+      </c>
+      <c r="AI27" s="2">
+        <v>20</v>
+      </c>
+      <c r="AJ27" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK27" s="2">
+        <v>20</v>
+      </c>
+      <c r="AL27" s="2">
+        <v>20</v>
+      </c>
+      <c r="AM27" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="17">
+        <v>272</v>
+      </c>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="8"/>
+      <c r="W28" s="8"/>
+      <c r="X28" s="8"/>
+      <c r="Y28" s="8"/>
+      <c r="Z28" s="8"/>
+      <c r="AA28" s="8"/>
+      <c r="AB28" s="8"/>
+      <c r="AC28" s="8"/>
+      <c r="AD28" s="8"/>
+      <c r="AE28" s="8"/>
+      <c r="AF28" s="8"/>
+      <c r="AG28" s="8"/>
+      <c r="AH28" s="8"/>
+      <c r="AI28" s="8"/>
+      <c r="AJ28" s="8"/>
+      <c r="AK28" s="8"/>
+      <c r="AL28" s="8"/>
+      <c r="AM28" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="14">
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="B25:B28"/>
     <mergeCell ref="A13:A16"/>
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="A1:A4"/>

</xml_diff>